<commit_message>
introduced guest account and handling
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -413,10 +413,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -525,7 +525,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>28</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>gast</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -539,7 +554,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -802,6 +817,584 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>4ot355g53h</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>rick</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2025-09-11T16:37:34.569542</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>4ot355g53h</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>rick</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2025-09-11T16:45:03.859558</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>4ot355g53h</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>rick</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2025-09-11T16:45:04.634407</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>gast</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2025-09-11T16:46:44.827159</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>gast</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2025-09-11T16:46:48.256704</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>gast</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2025-09-11T16:46:49.158282</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>gast</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2025-09-11T16:46:50.935001</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>4ot355g53h</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>rick</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2025-09-11T16:47:04.566519</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>4ot355g53h</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>rick</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2025-09-11T16:47:06.544106</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>4ot355g53h</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>rick</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2025-09-11T16:48:57.691330</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>4ot355g53h</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>rick</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2025-09-11T17:01:16.929735</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>4ot355g53h</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>rick</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2025-09-11T17:01:19.997282</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>4ot355g53h</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>rick</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2025-09-11T17:01:21.817021</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>4ot355g53h</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>rick</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2025-09-11T17:01:24.021084</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>4ot355g53h</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>rick</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2025-09-11T17:01:24.335717</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>4ot355g53h</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>rick</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>2025-09-11T17:01:24.530092</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>4ot355g53h</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>rick</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2025-09-11T17:01:26.602666</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>4ot355g53h</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>rick</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>2025-09-11T17:01:26.774413</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>4ot355g53h</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>rick</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2025-09-11T17:01:26.946217</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>4ot355g53h</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>rick</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>2025-09-11T17:01:28.218388</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>4ot355g53h</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>rick</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>2025-09-11T17:10:08.959011</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>4ot355g53h</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>rick</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>2025-09-11T17:10:09.711290</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>gast</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2025-09-11T17:10:11.195980</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>gast</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2025-09-11T17:10:12.205959</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>gast</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2025-09-11T17:10:12.782371</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>gast</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>2025-09-11T17:10:14.044459</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>4ot355g53h</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>rick</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>2025-09-11T17:10:15.672224</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>4ot355g53h</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>rick</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>2025-09-11T17:10:15.877200</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>gast</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>2025-09-11T17:17:26.899329</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>gast</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>2025-09-11T17:23:14.373956</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>gast</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>2025-09-11T17:23:14.870656</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>gast</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>2025-09-11T17:23:15.082736</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>gast</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>2025-09-11T17:23:15.409804</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>4ot355g53h</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>rick</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>2025-09-11T17:23:17.129687</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>